<commit_message>
Big Update 30 Jan 2022
</commit_message>
<xml_diff>
--- a/public/uploads/Persediaan Material.xlsx
+++ b/public/uploads/Persediaan Material.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Website Projects\My Projects\portal-pltd-kotamobagu\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE63E68-7D92-4C97-A238-B7B97FDFC0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54FA474-C5D7-40D4-844F-4F35C3D6CCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24540CD5-5C54-4E21-8382-E29A9A96FEB5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>descMat</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>hargaSat</t>
-  </si>
-  <si>
-    <t>totHarga</t>
   </si>
   <si>
     <t>000000003120228</t>
@@ -492,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C863912-EB2B-4CCD-B65B-C425962BF2E4}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D1" sqref="D1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +501,7 @@
     <col min="2" max="2" width="40.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -520,59 +517,50 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -580,39 +568,33 @@
       <c r="E4">
         <v>768768</v>
       </c>
-      <c r="F4">
-        <v>3075072</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -620,39 +602,33 @@
       <c r="E6">
         <v>1666500</v>
       </c>
-      <c r="F6">
-        <v>6666000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -660,19 +636,16 @@
       <c r="E8">
         <v>2120580</v>
       </c>
-      <c r="F8">
-        <v>4241160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -680,19 +653,16 @@
       <c r="E9">
         <v>1547150</v>
       </c>
-      <c r="F9">
-        <v>6188600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -700,19 +670,16 @@
       <c r="E10">
         <v>1094000</v>
       </c>
-      <c r="F10">
-        <v>1094000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -720,19 +687,16 @@
       <c r="E11">
         <v>777266</v>
       </c>
-      <c r="F11">
-        <v>3109065</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -740,19 +704,16 @@
       <c r="E12">
         <v>2112660</v>
       </c>
-      <c r="F12">
-        <v>8450640</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -760,19 +721,16 @@
       <c r="E13">
         <v>730840</v>
       </c>
-      <c r="F13">
-        <v>1461680</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -780,27 +738,21 @@
       <c r="E14">
         <v>1333750</v>
       </c>
-      <c r="F14">
-        <v>1333750</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
         <v>0</v>
       </c>
     </row>

</xml_diff>